<commit_message>
excel import data peserta
</commit_message>
<xml_diff>
--- a/assets/website/template/upload_peserta/Template_Upload_Peserta.xlsx
+++ b/assets/website/template/upload_peserta/Template_Upload_Peserta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\cbt\assets\website\template\upload_peserta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56BFD7BB-4E5E-420E-B054-C90CFE51EC9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D84489C3-E6CD-4D6C-B44E-8FADFD37B89A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{EA5C0B6E-E3CE-4991-9EE7-1AF17C3AF153}"/>
   </bookViews>
@@ -577,8 +577,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>